<commit_message>
Modified Factory class to manage schema.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -6,10 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schema" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delta" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delta1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delta2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +15,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Foreign Sheet</t>
+  </si>
+  <si>
+    <t>Foreign Key</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
   <si>
     <t>prop_a</t>
   </si>
@@ -361,14 +383,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -379,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,13 +468,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -405,6 +484,9 @@
       <c r="B2" t="n">
         <v>2</v>
       </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="n">
@@ -413,6 +495,9 @@
       <c r="B3" t="n">
         <v>2</v>
       </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="n">
@@ -421,6 +506,9 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="n">
@@ -429,6 +517,9 @@
       <c r="B5" t="n">
         <v>2</v>
       </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="n">
@@ -437,6 +528,9 @@
       <c r="B6" t="n">
         <v>2</v>
       </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="n">
@@ -445,113 +539,8 @@
       <c r="B7" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
+      <c r="C7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>